<commit_message>
update the latency algorithm, improve reliability
</commit_message>
<xml_diff>
--- a/profile_data/lightgbm/nx1.xlsx
+++ b/profile_data/lightgbm/nx1.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="4">
   <si>
     <t xml:space="preserve">t0</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">t2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t3</t>
   </si>
 </sst>
 </file>
@@ -68,7 +71,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -79,6 +82,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -116,7 +125,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -127,6 +136,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -146,13 +163,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="6:6"/>
+      <selection pane="topLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -165,22 +182,43 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>2</v>
+      <c r="J1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -191,24 +229,45 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="E2" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="F2" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="n">
-        <v>2</v>
-      </c>
       <c r="G2" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="M2" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="H2" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="I2" s="2" t="n">
+      <c r="N2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="O2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="P2" s="2" t="n">
         <v>7</v>
       </c>
     </row>
@@ -220,24 +279,45 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="E3" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="n">
-        <v>14</v>
-      </c>
       <c r="F3" s="2" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G3" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="M3" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="H3" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="I3" s="2" t="n">
+      <c r="N3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="O3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="P3" s="2" t="n">
         <v>8</v>
       </c>
     </row>
@@ -249,24 +329,45 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="n">
-        <v>13</v>
-      </c>
       <c r="E4" s="2" t="n">
         <v>13</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G4" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="L4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="H4" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="I4" s="2" t="n">
+      <c r="N4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="O4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="P4" s="2" t="n">
         <v>8</v>
       </c>
     </row>
@@ -278,24 +379,45 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>6</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>5</v>
       </c>
       <c r="G5" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I5" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="H5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2" t="n">
+      <c r="J5" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="M5" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="N5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" s="2" t="n">
         <v>5</v>
       </c>
     </row>
@@ -307,10 +429,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>3</v>
@@ -319,14 +441,53 @@
         <v>3</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I6" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" s="2" t="n">
         <v>0</v>
       </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -344,13 +505,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="6:6"/>
+      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -363,22 +524,43 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>2</v>
+      <c r="J1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -389,24 +571,45 @@
         <v>14</v>
       </c>
       <c r="C2" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="E2" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="E2" s="2" t="n">
-        <v>14</v>
-      </c>
       <c r="F2" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="I2" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="M2" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="N2" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="O2" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="P2" s="2" t="n">
         <v>7</v>
       </c>
     </row>
@@ -418,24 +621,45 @@
         <v>16</v>
       </c>
       <c r="C3" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="E3" s="2" t="n">
         <v>48</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="F3" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="G3" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H3" s="2" t="n">
         <v>36</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="I3" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="M3" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="N3" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="O3" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="P3" s="2" t="n">
         <v>8</v>
       </c>
     </row>
@@ -447,24 +671,45 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="E4" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="E4" s="2" t="n">
-        <v>13</v>
-      </c>
       <c r="F4" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="H4" s="2" t="n">
         <v>31</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="I4" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="L4" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="M4" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="H4" s="2" t="n">
-        <v>13</v>
-      </c>
-      <c r="I4" s="2" t="n">
+      <c r="N4" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="O4" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="P4" s="2" t="n">
         <v>7</v>
       </c>
     </row>
@@ -476,24 +721,45 @@
         <v>16</v>
       </c>
       <c r="C5" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="E5" s="2" t="n">
         <v>49</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="F5" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F5" s="2" t="n">
-        <v>14</v>
-      </c>
       <c r="G5" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="M5" s="2" t="n">
         <v>43</v>
       </c>
-      <c r="H5" s="2" t="n">
-        <v>14</v>
-      </c>
-      <c r="I5" s="2" t="n">
+      <c r="N5" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="O5" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="P5" s="2" t="n">
         <v>9</v>
       </c>
     </row>
@@ -505,28 +771,70 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>3</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>3</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>3</v>
       </c>
+      <c r="J6" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="O6" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A7:D7"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -545,10 +853,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="6:6 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -568,10 +876,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="6:6 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -591,10 +899,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="6:6 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -614,10 +922,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="6:6 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -637,10 +945,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="6:6 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>